<commit_message>
near to the end !
</commit_message>
<xml_diff>
--- a/otchet.xlsx
+++ b/otchet.xlsx
@@ -46,11 +46,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -492,10 +493,35 @@
     </row>
     <row r="4"/>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>awd</t>
-        </is>
+      <c r="A5" s="1" t="n"/>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>Direct Flight</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5591</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>09AUG22-11AUG22</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>.2.4...</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.4791666666666667</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.5590277777777778</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6"/>

</xml_diff>